<commit_message>
added wireframes and updated moscow
</commit_message>
<xml_diff>
--- a/documentation/moscow_protask.xlsx
+++ b/documentation/moscow_protask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31620\Documents\Github\rock-paper-code\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E7E03-9633-423D-B3BD-097426665658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89384686-382E-4148-BC96-69BA9A3EF3C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{BEA3FCAD-9ABF-494F-B1D0-982A820D19EC}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>text based rock paper scissors</t>
   </si>
   <si>
-    <t>picture based rock paper scissors</t>
-  </si>
-  <si>
     <t>difficulty select between easy, random and impossible AI</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>live feed rock paper scissors with pictures</t>
+  </si>
+  <si>
+    <t>Color recognicion rock paper scissors</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,47 +477,47 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>